<commit_message>
tentativas de melhoria na divisao silabica
</commit_message>
<xml_diff>
--- a/files/pseudoPalavras.xlsx
+++ b/files/pseudoPalavras.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>palavra</t>
   </si>
@@ -25,91 +25,46 @@
     <t>tonicidade</t>
   </si>
   <si>
-    <t>dipadê</t>
-  </si>
-  <si>
-    <t>pigidê</t>
-  </si>
-  <si>
-    <t>xepacá</t>
-  </si>
-  <si>
-    <t>cagecá</t>
-  </si>
-  <si>
-    <t>cegecá</t>
-  </si>
-  <si>
-    <t>supatá</t>
-  </si>
-  <si>
-    <t>mapitá</t>
-  </si>
-  <si>
-    <t>xeritá</t>
-  </si>
-  <si>
-    <t>gaparimatá</t>
-  </si>
-  <si>
-    <t>nidirepitá</t>
-  </si>
-  <si>
-    <t>xecapigitá</t>
-  </si>
-  <si>
-    <t>rigaxeretá</t>
-  </si>
-  <si>
-    <t>regená</t>
-  </si>
-  <si>
-    <t>cadiná</t>
-  </si>
-  <si>
-    <t>sudiná</t>
-  </si>
-  <si>
-    <t>rozaná</t>
-  </si>
-  <si>
-    <t>pimaná</t>
-  </si>
-  <si>
-    <t>xedirirá</t>
-  </si>
-  <si>
-    <t>rocanirá</t>
-  </si>
-  <si>
-    <t>sugadirá</t>
-  </si>
-  <si>
-    <t>gecazará</t>
-  </si>
-  <si>
-    <t>macerá</t>
-  </si>
-  <si>
-    <t>camará</t>
-  </si>
-  <si>
-    <t>rerirá</t>
-  </si>
-  <si>
-    <t>roxeripará</t>
-  </si>
-  <si>
-    <t>dipigapará</t>
-  </si>
-  <si>
-    <t>sugizapirá</t>
-  </si>
-  <si>
-    <t>gedicarirá</t>
-  </si>
-  <si>
-    <t>cagixedirá</t>
+    <t>capuzar</t>
+  </si>
+  <si>
+    <t>soscapzar</t>
+  </si>
+  <si>
+    <t>tarozar</t>
+  </si>
+  <si>
+    <t>tasosroseu</t>
+  </si>
+  <si>
+    <t>rogavaniu</t>
+  </si>
+  <si>
+    <t>sosvagaporu</t>
+  </si>
+  <si>
+    <t>gatuserou</t>
+  </si>
+  <si>
+    <t>gotará</t>
+  </si>
+  <si>
+    <t>eszarrá</t>
+  </si>
+  <si>
+    <t>orsepor</t>
+  </si>
+  <si>
+    <t>esvapor</t>
+  </si>
+  <si>
+    <t>esporcaporu</t>
+  </si>
+  <si>
+    <t>uorsosporu</t>
+  </si>
+  <si>
+    <t>serogasosu</t>
   </si>
   <si>
     <t>oxítona</t>
@@ -470,7 +425,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -495,10 +450,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>32</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -509,10 +461,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>32</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -523,10 +472,7 @@
         <v>5</v>
       </c>
       <c r="C4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>32</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -537,10 +483,7 @@
         <v>6</v>
       </c>
       <c r="C5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>32</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -551,10 +494,7 @@
         <v>7</v>
       </c>
       <c r="C6" t="b">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
-        <v>32</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -565,10 +505,7 @@
         <v>8</v>
       </c>
       <c r="C7" t="b">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>32</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -579,10 +516,7 @@
         <v>9</v>
       </c>
       <c r="C8" t="b">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
-        <v>32</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -596,7 +530,7 @@
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -607,10 +541,7 @@
         <v>11</v>
       </c>
       <c r="C10" t="b">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>32</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -621,10 +552,7 @@
         <v>12</v>
       </c>
       <c r="C11" t="b">
-        <v>1</v>
-      </c>
-      <c r="D11" t="s">
-        <v>32</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -635,10 +563,7 @@
         <v>13</v>
       </c>
       <c r="C12" t="b">
-        <v>1</v>
-      </c>
-      <c r="D12" t="s">
-        <v>32</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -649,10 +574,7 @@
         <v>14</v>
       </c>
       <c r="C13" t="b">
-        <v>1</v>
-      </c>
-      <c r="D13" t="s">
-        <v>32</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -663,10 +585,7 @@
         <v>15</v>
       </c>
       <c r="C14" t="b">
-        <v>1</v>
-      </c>
-      <c r="D14" t="s">
-        <v>32</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -680,217 +599,7 @@
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="1">
-        <v>14</v>
-      </c>
-      <c r="B16" t="s">
         <v>17</v>
-      </c>
-      <c r="C16" t="b">
-        <v>1</v>
-      </c>
-      <c r="D16" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="1">
-        <v>15</v>
-      </c>
-      <c r="B17" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" t="b">
-        <v>1</v>
-      </c>
-      <c r="D17" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="1">
-        <v>16</v>
-      </c>
-      <c r="B18" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" t="b">
-        <v>1</v>
-      </c>
-      <c r="D18" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="1">
-        <v>17</v>
-      </c>
-      <c r="B19" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19" t="b">
-        <v>1</v>
-      </c>
-      <c r="D19" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="1">
-        <v>18</v>
-      </c>
-      <c r="B20" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" t="b">
-        <v>1</v>
-      </c>
-      <c r="D20" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="1">
-        <v>19</v>
-      </c>
-      <c r="B21" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21" t="b">
-        <v>1</v>
-      </c>
-      <c r="D21" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="1">
-        <v>20</v>
-      </c>
-      <c r="B22" t="s">
-        <v>23</v>
-      </c>
-      <c r="C22" t="b">
-        <v>1</v>
-      </c>
-      <c r="D22" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="1">
-        <v>21</v>
-      </c>
-      <c r="B23" t="s">
-        <v>24</v>
-      </c>
-      <c r="C23" t="b">
-        <v>1</v>
-      </c>
-      <c r="D23" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="1">
-        <v>22</v>
-      </c>
-      <c r="B24" t="s">
-        <v>25</v>
-      </c>
-      <c r="C24" t="b">
-        <v>1</v>
-      </c>
-      <c r="D24" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="1">
-        <v>23</v>
-      </c>
-      <c r="B25" t="s">
-        <v>26</v>
-      </c>
-      <c r="C25" t="b">
-        <v>1</v>
-      </c>
-      <c r="D25" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="1">
-        <v>24</v>
-      </c>
-      <c r="B26" t="s">
-        <v>27</v>
-      </c>
-      <c r="C26" t="b">
-        <v>1</v>
-      </c>
-      <c r="D26" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="1">
-        <v>25</v>
-      </c>
-      <c r="B27" t="s">
-        <v>28</v>
-      </c>
-      <c r="C27" t="b">
-        <v>1</v>
-      </c>
-      <c r="D27" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="1">
-        <v>26</v>
-      </c>
-      <c r="B28" t="s">
-        <v>29</v>
-      </c>
-      <c r="C28" t="b">
-        <v>1</v>
-      </c>
-      <c r="D28" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="1">
-        <v>27</v>
-      </c>
-      <c r="B29" t="s">
-        <v>30</v>
-      </c>
-      <c r="C29" t="b">
-        <v>1</v>
-      </c>
-      <c r="D29" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="1">
-        <v>28</v>
-      </c>
-      <c r="B30" t="s">
-        <v>31</v>
-      </c>
-      <c r="C30" t="b">
-        <v>1</v>
-      </c>
-      <c r="D30" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
*csv e *.xlsx adicionados ao .gitignore
</commit_message>
<xml_diff>
--- a/files/pseudoPalavras.xlsx
+++ b/files/pseudoPalavras.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="55">
   <si>
     <t>palavra</t>
   </si>
@@ -25,49 +25,160 @@
     <t>tonicidade</t>
   </si>
   <si>
-    <t>capuzar</t>
-  </si>
-  <si>
-    <t>soscapzar</t>
-  </si>
-  <si>
-    <t>tarozar</t>
-  </si>
-  <si>
-    <t>tasosroseu</t>
-  </si>
-  <si>
-    <t>rogavaniu</t>
-  </si>
-  <si>
-    <t>sosvagaporu</t>
-  </si>
-  <si>
-    <t>gatuserou</t>
-  </si>
-  <si>
-    <t>gotará</t>
-  </si>
-  <si>
-    <t>eszarrá</t>
-  </si>
-  <si>
-    <t>orsepor</t>
-  </si>
-  <si>
-    <t>esvapor</t>
-  </si>
-  <si>
-    <t>esporcaporu</t>
-  </si>
-  <si>
-    <t>uorsosporu</t>
-  </si>
-  <si>
-    <t>serogasosu</t>
-  </si>
-  <si>
-    <t>oxítona</t>
+    <t>erocapucasçásemos</t>
+  </si>
+  <si>
+    <t>mastonospicoçáseun</t>
+  </si>
+  <si>
+    <t>vamosgitopiçáati</t>
+  </si>
+  <si>
+    <t>ciputeosmóseto</t>
+  </si>
+  <si>
+    <t>gitofinimótepu</t>
+  </si>
+  <si>
+    <t>dicodaunmónici</t>
+  </si>
+  <si>
+    <t>picosfigomólanos</t>
+  </si>
+  <si>
+    <t>üilomasorsêxvala</t>
+  </si>
+  <si>
+    <t>aervinisêxcasgi</t>
+  </si>
+  <si>
+    <t>osocpicrécosun</t>
+  </si>
+  <si>
+    <t>osnificrénosci</t>
+  </si>
+  <si>
+    <t>tipugicrécosci</t>
+  </si>
+  <si>
+    <t>mosvatipudécaos</t>
+  </si>
+  <si>
+    <t>tigimasmosdétela</t>
+  </si>
+  <si>
+    <t>vacodanidétepu</t>
+  </si>
+  <si>
+    <t>vaerortodépica</t>
+  </si>
+  <si>
+    <t>latuptolímcooc</t>
+  </si>
+  <si>
+    <t>masdamoslímdior</t>
+  </si>
+  <si>
+    <t>amascaslímfios</t>
+  </si>
+  <si>
+    <t>tuposcaráocmos</t>
+  </si>
+  <si>
+    <t>pigierráteoc</t>
+  </si>
+  <si>
+    <t>casmosüiráorpi</t>
+  </si>
+  <si>
+    <t>masüimosrácaci</t>
+  </si>
+  <si>
+    <t>secasarátupun</t>
+  </si>
+  <si>
+    <t>pufiditámasgo</t>
+  </si>
+  <si>
+    <t>toorvatágica</t>
+  </si>
+  <si>
+    <t>lafipupicicrôdise</t>
+  </si>
+  <si>
+    <t>osdafivicascrôtiun</t>
+  </si>
+  <si>
+    <t>vimasocpóvate</t>
+  </si>
+  <si>
+    <t>gipivapómosse</t>
+  </si>
+  <si>
+    <t>costuposcaüiórtidi</t>
+  </si>
+  <si>
+    <t>gimoscanosgoórdiüi</t>
+  </si>
+  <si>
+    <t>maslaticostupórseva</t>
+  </si>
+  <si>
+    <t>daselaüitocráospi</t>
+  </si>
+  <si>
+    <t>undateniorcrácipu</t>
+  </si>
+  <si>
+    <t>orpucascaoscráocgi</t>
+  </si>
+  <si>
+    <t>erpiatoüicráosco</t>
+  </si>
+  <si>
+    <t>avicasergicrápila</t>
+  </si>
+  <si>
+    <t>locamosmastógite</t>
+  </si>
+  <si>
+    <t>titofioctóüier</t>
+  </si>
+  <si>
+    <t>unvifigotócoer</t>
+  </si>
+  <si>
+    <t>gicapiráseüi</t>
+  </si>
+  <si>
+    <t>casoslaráora</t>
+  </si>
+  <si>
+    <t>totenirágia</t>
+  </si>
+  <si>
+    <t>vicasmascosfríocpi</t>
+  </si>
+  <si>
+    <t>uncitupcasfríerfi</t>
+  </si>
+  <si>
+    <t>orcounmasfríüito</t>
+  </si>
+  <si>
+    <t>cosatupnosséqdite</t>
+  </si>
+  <si>
+    <t>vatupertoséqpucas</t>
+  </si>
+  <si>
+    <t>givituperséqtolo</t>
+  </si>
+  <si>
+    <t>pigierunséqcaci</t>
+  </si>
+  <si>
+    <t>proparoxítona</t>
   </si>
 </sst>
 </file>
@@ -425,7 +536,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -494,7 +605,10 @@
         <v>7</v>
       </c>
       <c r="C6" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -527,10 +641,7 @@
         <v>10</v>
       </c>
       <c r="C9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D9" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -596,10 +707,420 @@
         <v>16</v>
       </c>
       <c r="C15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" t="b">
         <v>1</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="1">
         <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="1">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="1">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="1">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>31</v>
+      </c>
+      <c r="C30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="1">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="1">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="1">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>34</v>
+      </c>
+      <c r="C33" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="1">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>35</v>
+      </c>
+      <c r="C34" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="1">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>36</v>
+      </c>
+      <c r="C35" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="1">
+        <v>34</v>
+      </c>
+      <c r="B36" t="s">
+        <v>37</v>
+      </c>
+      <c r="C36" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="1">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>38</v>
+      </c>
+      <c r="C37" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="1">
+        <v>36</v>
+      </c>
+      <c r="B38" t="s">
+        <v>39</v>
+      </c>
+      <c r="C38" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="1">
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
+        <v>40</v>
+      </c>
+      <c r="C39" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="1">
+        <v>38</v>
+      </c>
+      <c r="B40" t="s">
+        <v>41</v>
+      </c>
+      <c r="C40" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="1">
+        <v>39</v>
+      </c>
+      <c r="B41" t="s">
+        <v>42</v>
+      </c>
+      <c r="C41" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="1">
+        <v>40</v>
+      </c>
+      <c r="B42" t="s">
+        <v>43</v>
+      </c>
+      <c r="C42" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="1">
+        <v>41</v>
+      </c>
+      <c r="B43" t="s">
+        <v>44</v>
+      </c>
+      <c r="C43" t="b">
+        <v>1</v>
+      </c>
+      <c r="D43" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="1">
+        <v>42</v>
+      </c>
+      <c r="B44" t="s">
+        <v>45</v>
+      </c>
+      <c r="C44" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="1">
+        <v>43</v>
+      </c>
+      <c r="B45" t="s">
+        <v>46</v>
+      </c>
+      <c r="C45" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="1">
+        <v>44</v>
+      </c>
+      <c r="B46" t="s">
+        <v>47</v>
+      </c>
+      <c r="C46" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="1">
+        <v>45</v>
+      </c>
+      <c r="B47" t="s">
+        <v>48</v>
+      </c>
+      <c r="C47" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="1">
+        <v>46</v>
+      </c>
+      <c r="B48" t="s">
+        <v>49</v>
+      </c>
+      <c r="C48" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="1">
+        <v>47</v>
+      </c>
+      <c r="B49" t="s">
+        <v>50</v>
+      </c>
+      <c r="C49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="1">
+        <v>48</v>
+      </c>
+      <c r="B50" t="s">
+        <v>51</v>
+      </c>
+      <c r="C50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="1">
+        <v>49</v>
+      </c>
+      <c r="B51" t="s">
+        <v>52</v>
+      </c>
+      <c r="C51" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="1">
+        <v>50</v>
+      </c>
+      <c r="B52" t="s">
+        <v>53</v>
+      </c>
+      <c r="C52" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>